<commit_message>
convert competitor to athlete
</commit_message>
<xml_diff>
--- a/docu/C2_Tables.xlsx
+++ b/docu/C2_Tables.xlsx
@@ -81,9 +81,6 @@
     <t>competition</t>
   </si>
   <si>
-    <t>competitor</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>tableauLink</t>
+  </si>
+  <si>
+    <t>athlete</t>
   </si>
 </sst>
 </file>
@@ -367,10 +367,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -668,7 +668,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -703,7 +703,7 @@
       <c r="B3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:14">
       <c r="B4" s="1" t="s">
@@ -716,7 +716,7 @@
         <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -730,10 +730,10 @@
         <v>20</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="7"/>
@@ -746,13 +746,13 @@
         <v>4</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L6" s="11"/>
       <c r="N6" s="11"/>
@@ -765,13 +765,13 @@
         <v>5</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L7" s="9"/>
       <c r="N7" s="10"/>
@@ -784,69 +784,69 @@
         <v>6</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:14">
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9" s="9"/>
       <c r="N9" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L10" s="9"/>
       <c r="N10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="17"/>
       <c r="E11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="17"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="N11" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="N12" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="17"/>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:14">
@@ -854,7 +854,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L14" s="13"/>
     </row>
@@ -863,12 +863,12 @@
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
       <c r="I15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L15" s="13"/>
     </row>
@@ -877,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="13"/>
@@ -890,28 +890,28 @@
       <c r="E17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="16"/>
       <c r="I17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="2:13">
       <c r="I18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="17"/>
       <c r="E19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="17"/>
       <c r="I19" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -931,13 +931,13 @@
       <c r="B21" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="16"/>
+      <c r="C21" s="17"/>
       <c r="E21" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="17"/>
       <c r="I21" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
@@ -949,7 +949,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
@@ -958,9 +958,9 @@
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
+      <c r="C23" s="17"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
+      <c r="F23" s="17"/>
       <c r="I23" s="9"/>
       <c r="J23" s="13"/>
     </row>
@@ -971,19 +971,19 @@
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="C25" s="17"/>
       <c r="E25" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="16"/>
+        <v>40</v>
+      </c>
+      <c r="F25" s="17"/>
       <c r="I25" s="10"/>
       <c r="J25" s="13"/>
     </row>
     <row r="26" spans="2:13">
       <c r="C26" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J26" s="13"/>
     </row>
@@ -995,19 +995,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>